<commit_message>
test upload commit of changes to excel file
</commit_message>
<xml_diff>
--- a/v2plus_reorganization/test.xlsx
+++ b/v2plus_reorganization/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrf/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD38C2FF-B0FD-CA42-9F0F-060DDCA1AA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8236B61-CB79-D640-AD7B-BB2D4383B229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="8000" windowWidth="27240" windowHeight="16440" xr2:uid="{DEF265A9-2FC8-7A4F-AEDD-BCEDFEE6A87B}"/>
+    <workbookView xWindow="12420" yWindow="8460" windowWidth="27240" windowHeight="16440" xr2:uid="{DEF265A9-2FC8-7A4F-AEDD-BCEDFEE6A87B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>test</t>
+    <t>test with changes</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027617C5-3A38-E14C-9E50-4CCD06B16FAC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>